<commit_message>
Change column number <-> colour
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -394,16 +394,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="20"/>
-    <col customWidth="1" max="3" min="3" width="12"/>
+    <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="5" min="5" width="34"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="30" r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Nazwa firmy</t>
-        </is>
-      </c>
+      <c r="A1" s="1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -418,12 +414,12 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
+          <t>Ilość</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
           <t>Rodzaj</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>Ilość</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -440,210 +436,32 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
           <t>styropian</t>
-        </is>
-      </c>
-      <c r="D3" s="5" t="inlineStr">
-        <is>
-          <t>12</t>
         </is>
       </c>
       <c r="E3" s="6" t="n"/>
     </row>
-    <row r="4">
-      <c r="A4" s="6" t="n"/>
-      <c r="B4" s="6" t="n"/>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>czarny</t>
-        </is>
-      </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E4" s="6" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="n"/>
-      <c r="B5" s="6" t="n"/>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>bialy</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
-      </c>
-      <c r="E5" s="6" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="n"/>
-      <c r="B6" s="6" t="n"/>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>ecru</t>
-        </is>
-      </c>
-      <c r="D6" s="5" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>M3</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>163</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>styropian</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="E7" s="6" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="n"/>
-      <c r="B8" s="6" t="n"/>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>czarny</t>
-        </is>
-      </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
-      </c>
-      <c r="E8" s="6" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="n"/>
-      <c r="B9" s="6" t="n"/>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t>bialy</t>
-        </is>
-      </c>
-      <c r="D9" s="5" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="E9" s="6" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="n"/>
-      <c r="B10" s="6" t="n"/>
-      <c r="C10" s="5" t="inlineStr">
-        <is>
-          <t>ecru</t>
-        </is>
-      </c>
-      <c r="D10" s="5" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="E10" s="6" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="n"/>
-      <c r="B11" s="6" t="n"/>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>czerwony</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
-      </c>
-      <c r="E11" s="6" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="inlineStr">
-        <is>
-          <t>Statyw drewniany</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>76</t>
-        </is>
-      </c>
-      <c r="C12" s="5" t="inlineStr">
-        <is>
-          <t>biały</t>
-        </is>
-      </c>
-      <c r="D12" s="5" t="inlineStr">
-        <is>
-          <t>76</t>
-        </is>
-      </c>
-      <c r="E12" s="6" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="inlineStr">
-        <is>
-          <t>Statyw metalowy</t>
-        </is>
-      </c>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
-      </c>
-      <c r="D13" s="5" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E13" s="6" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="n"/>
-      <c r="B14" s="6" t="n"/>
-      <c r="C14" s="5" t="inlineStr">
-        <is>
-          <t>Ślimak</t>
-        </is>
-      </c>
-      <c r="D14" s="5" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E14" s="6" t="n"/>
-    </row>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
     <row r="15"/>
     <row r="16"/>
     <row r="17"/>
@@ -668,16 +486,10 @@
     <row r="36"/>
     <row r="37"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B12"/>
-    <mergeCell ref="A12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B3"/>
+    <mergeCell ref="A3"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve PDFgen - fixed to work with simple products objects
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -399,7 +399,11 @@
   </cols>
   <sheetData>
     <row customHeight="1" ht="30" r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>dupa</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -431,18 +435,16 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>M1</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>12</v>
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
@@ -451,11 +453,95 @@
       </c>
       <c r="E3" s="6" t="n"/>
     </row>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
+    <row r="4">
+      <c r="A4" s="6" t="n"/>
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>bialy</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>D9</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>styropian</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Statyw drewniany</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>biały</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Statyw metalowy</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n"/>
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="n"/>
+    </row>
     <row r="9"/>
     <row r="10"/>
     <row r="11"/>
@@ -486,10 +572,16 @@
     <row r="36"/>
     <row r="37"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B3"/>
-    <mergeCell ref="A3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B5"/>
+    <mergeCell ref="A5"/>
+    <mergeCell ref="B6"/>
+    <mergeCell ref="A6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Rebuiiding order: rebuilding dummys done (with some small bugs)
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,9 +32,6 @@
     <font>
       <b val="1"/>
       <sz val="18"/>
-    </font>
-    <font>
-      <sz val="14"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,22 +69,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -399,11 +386,7 @@
   </cols>
   <sheetData>
     <row customHeight="1" ht="30" r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>dupa</t>
-        </is>
-      </c>
+      <c r="A1" s="1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -432,116 +415,12 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>M3</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t>styropian</t>
-        </is>
-      </c>
-      <c r="E3" s="6" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="n"/>
-      <c r="B4" s="6" t="n"/>
-      <c r="C4" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>bialy</t>
-        </is>
-      </c>
-      <c r="E4" s="6" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>D9</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>styropian</t>
-        </is>
-      </c>
-      <c r="E5" s="6" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>Statyw drewniany</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>biały</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>Statyw metalowy</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
-      </c>
-      <c r="E7" s="6" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="n"/>
-      <c r="B8" s="6" t="n"/>
-      <c r="C8" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="D8" s="4" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="E8" s="6" t="n"/>
-    </row>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
     <row r="9"/>
     <row r="10"/>
     <row r="11"/>
@@ -572,16 +451,8 @@
     <row r="36"/>
     <row r="37"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B5"/>
-    <mergeCell ref="A5"/>
-    <mergeCell ref="B6"/>
-    <mergeCell ref="A6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
First part of basicProduct class done - class to simplify other products class using inheriting
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,6 +32,9 @@
     <font>
       <b val="1"/>
       <sz val="18"/>
+    </font>
+    <font>
+      <sz val="14"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,12 +72,22 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -415,10 +428,74 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>czarny</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n"/>
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>czarny</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="n"/>
+      <c r="B5" s="6" t="n"/>
+      <c r="C5" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>bialy</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>styropian</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="n"/>
+    </row>
     <row r="7"/>
     <row r="8"/>
     <row r="9"/>
@@ -451,8 +528,12 @@
     <row r="36"/>
     <row r="37"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B6"/>
+    <mergeCell ref="A6"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Start changing PDFgen class, add methods of geting data from basicProducts classes
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -399,7 +399,11 @@
   </cols>
   <sheetData>
     <row customHeight="1" ht="30" r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>fimra01</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -431,20 +435,16 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>D2</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="n"/>
       <c r="C3" s="5" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t>czarny</t>
+          <t>styropian</t>
         </is>
       </c>
       <c r="E3" s="6" t="n"/>
@@ -453,7 +453,7 @@
       <c r="A4" s="6" t="n"/>
       <c r="B4" s="6" t="n"/>
       <c r="C4" s="5" t="n">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
@@ -478,16 +478,12 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>M1</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="n"/>
       <c r="C6" s="5" t="n">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
@@ -496,11 +492,79 @@
       </c>
       <c r="E6" s="6" t="n"/>
     </row>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
+    <row r="7">
+      <c r="A7" s="6" t="n"/>
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>czarny</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>woodenStands</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n"/>
+      <c r="C8" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>biały</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n"/>
+      <c r="B9" s="6" t="n"/>
+      <c r="C9" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>czarny</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>stands</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="n"/>
+      <c r="C10" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n"/>
+      <c r="B11" s="6" t="n"/>
+      <c r="C11" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="n"/>
+    </row>
     <row r="12"/>
     <row r="13"/>
     <row r="14"/>
@@ -528,12 +592,16 @@
     <row r="36"/>
     <row r="37"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B6"/>
-    <mergeCell ref="A6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add sum calculate method in orderManager, add sum to PDF, and change model source(PDF)
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -438,7 +438,9 @@
           <t>M1</t>
         </is>
       </c>
-      <c r="B3" s="4" t="n"/>
+      <c r="B3" s="4" t="n">
+        <v>65</v>
+      </c>
       <c r="C3" s="5" t="n">
         <v>21</v>
       </c>
@@ -481,7 +483,9 @@
           <t>M3</t>
         </is>
       </c>
-      <c r="B6" s="4" t="n"/>
+      <c r="B6" s="4" t="n">
+        <v>44</v>
+      </c>
       <c r="C6" s="5" t="n">
         <v>12</v>
       </c>
@@ -508,10 +512,12 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>woodenStands</t>
-        </is>
-      </c>
-      <c r="B8" s="4" t="n"/>
+          <t>Statyw drewniany</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>55</v>
+      </c>
       <c r="C8" s="5" t="n">
         <v>33</v>
       </c>
@@ -538,10 +544,12 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>stands</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="n"/>
+          <t>Statyw metalowy</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>15</v>
+      </c>
       <c r="C10" s="5" t="n">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Add order and collect date in PDF generation
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,6 +32,9 @@
     <font>
       <b val="1"/>
       <sz val="18"/>
+    </font>
+    <font>
+      <sz val="12"/>
     </font>
     <font>
       <sz val="14"/>
@@ -72,22 +75,25 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -408,173 +414,195 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
+          <t>Data zamówienia:</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>22.4.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Data odbioru:</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>30.4.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Suma</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>Ilość</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>Rodzaj</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>Uwagi</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>M1</t>
         </is>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>65</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="D5" s="5" t="inlineStr">
         <is>
           <t>styropian</t>
         </is>
       </c>
-      <c r="E3" s="6" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="n"/>
-      <c r="B4" s="6" t="n"/>
-      <c r="C4" s="5" t="n">
+      <c r="E5" s="7" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="n"/>
+      <c r="B6" s="7" t="n"/>
+      <c r="C6" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="D4" s="4" t="inlineStr">
+      <c r="D6" s="5" t="inlineStr">
         <is>
           <t>czarny</t>
         </is>
       </c>
-      <c r="E4" s="6" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="n"/>
-      <c r="B5" s="6" t="n"/>
-      <c r="C5" s="5" t="n">
+      <c r="E6" s="7" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="n"/>
+      <c r="B7" s="7" t="n"/>
+      <c r="C7" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="inlineStr">
+      <c r="D7" s="5" t="inlineStr">
         <is>
           <t>bialy</t>
         </is>
       </c>
-      <c r="E5" s="6" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="E7" s="7" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>M3</t>
         </is>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="D6" s="4" t="inlineStr">
+      <c r="D8" s="5" t="inlineStr">
         <is>
           <t>styropian</t>
         </is>
       </c>
-      <c r="E6" s="6" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="n"/>
-      <c r="B7" s="6" t="n"/>
-      <c r="C7" s="5" t="n">
+      <c r="E8" s="7" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="n"/>
+      <c r="B9" s="7" t="n"/>
+      <c r="C9" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="D7" s="4" t="inlineStr">
+      <c r="D9" s="5" t="inlineStr">
         <is>
           <t>czarny</t>
         </is>
       </c>
-      <c r="E7" s="6" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="E9" s="7" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Statyw drewniany</t>
         </is>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B10" s="5" t="n">
         <v>55</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C10" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="D8" s="4" t="inlineStr">
+      <c r="D10" s="5" t="inlineStr">
         <is>
           <t>biały</t>
         </is>
       </c>
-      <c r="E8" s="6" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="n"/>
-      <c r="B9" s="6" t="n"/>
-      <c r="C9" s="5" t="n">
+      <c r="E10" s="7" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="n"/>
+      <c r="B11" s="7" t="n"/>
+      <c r="C11" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="D9" s="4" t="inlineStr">
+      <c r="D11" s="5" t="inlineStr">
         <is>
           <t>czarny</t>
         </is>
       </c>
-      <c r="E9" s="6" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="inlineStr">
+      <c r="E11" s="7" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Statyw metalowy</t>
         </is>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B12" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C12" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="D10" s="4" t="inlineStr">
+      <c r="D12" s="5" t="inlineStr">
         <is>
           <t>45</t>
         </is>
       </c>
-      <c r="E10" s="6" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="n"/>
-      <c r="B11" s="6" t="n"/>
-      <c r="C11" s="5" t="n">
+      <c r="E12" s="7" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="n"/>
+      <c r="B13" s="7" t="n"/>
+      <c r="C13" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="D11" s="4" t="inlineStr">
+      <c r="D13" s="5" t="inlineStr">
         <is>
           <t>90</t>
         </is>
       </c>
-      <c r="E11" s="6" t="n"/>
-    </row>
-    <row r="12"/>
-    <row r="13"/>
+      <c r="E13" s="7" t="n"/>
+    </row>
     <row r="14"/>
     <row r="15"/>
     <row r="16"/>
@@ -600,16 +628,18 @@
     <row r="36"/>
     <row r="37"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
II part improving PDF gen
-Show invoice and payment in PDF file
-Fix bug - when only one product type was in order
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -407,7 +407,7 @@
     <row customHeight="1" ht="30" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>fimra01</t>
+          <t>fizmasss</t>
         </is>
       </c>
     </row>
@@ -419,7 +419,17 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>22.4.2020</t>
+          <t>27.4.2020</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Nr faktury:</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>eX2137/20</t>
         </is>
       </c>
     </row>
@@ -431,8 +441,16 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>30.4.2020</t>
-        </is>
+          <t>27.4.2020</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Płatność:</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -469,10 +487,10 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
@@ -485,7 +503,7 @@
       <c r="A6" s="7" t="n"/>
       <c r="B6" s="7" t="n"/>
       <c r="C6" s="6" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
@@ -494,115 +512,13 @@
       </c>
       <c r="E6" s="7" t="n"/>
     </row>
-    <row r="7">
-      <c r="A7" s="7" t="n"/>
-      <c r="B7" s="7" t="n"/>
-      <c r="C7" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>bialy</t>
-        </is>
-      </c>
-      <c r="E7" s="7" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t>M3</t>
-        </is>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>styropian</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="n"/>
-      <c r="B9" s="7" t="n"/>
-      <c r="C9" s="6" t="n">
-        <v>32</v>
-      </c>
-      <c r="D9" s="5" t="inlineStr">
-        <is>
-          <t>czarny</t>
-        </is>
-      </c>
-      <c r="E9" s="7" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Statyw drewniany</t>
-        </is>
-      </c>
-      <c r="B10" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="C10" s="6" t="n">
-        <v>33</v>
-      </c>
-      <c r="D10" s="5" t="inlineStr">
-        <is>
-          <t>biały</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="7" t="n"/>
-      <c r="B11" s="7" t="n"/>
-      <c r="C11" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5" t="inlineStr">
-        <is>
-          <t>czarny</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Statyw metalowy</t>
-        </is>
-      </c>
-      <c r="B12" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="D12" s="5" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="E12" s="7" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="n"/>
-      <c r="B13" s="7" t="n"/>
-      <c r="C13" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
-      </c>
-      <c r="E13" s="7" t="n"/>
-    </row>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
     <row r="14"/>
     <row r="15"/>
     <row r="16"/>
@@ -628,18 +544,12 @@
     <row r="36"/>
     <row r="37"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
III part of improving PDF gen
- improve date generation
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -407,7 +407,7 @@
     <row customHeight="1" ht="30" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>fizmasss</t>
+          <t>fimra01</t>
         </is>
       </c>
     </row>
@@ -419,17 +419,17 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>27.4.2020</t>
+          <t>22.4.2020</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Nr faktury:</t>
+          <t xml:space="preserve">Nr faktury: </t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>eX2137/20</t>
+          <t>assdff123</t>
         </is>
       </c>
     </row>
@@ -441,16 +441,16 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>27.4.2020</t>
+          <t>30.4.2020</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>Płatność:</t>
+          <t xml:space="preserve">Płatność: </t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4">
@@ -487,10 +487,10 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
@@ -503,22 +503,124 @@
       <c r="A6" s="7" t="n"/>
       <c r="B6" s="7" t="n"/>
       <c r="C6" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>czarny</t>
+        </is>
+      </c>
+      <c r="E6" s="7" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="n"/>
+      <c r="B7" s="7" t="n"/>
+      <c r="C7" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>bialy</t>
+        </is>
+      </c>
+      <c r="E7" s="7" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>styropian</t>
+        </is>
+      </c>
+      <c r="E8" s="7" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="n"/>
+      <c r="B9" s="7" t="n"/>
+      <c r="C9" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>czarny</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>Statyw drewniany</t>
+        </is>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>55</v>
+      </c>
+      <c r="C10" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="D10" s="5" t="inlineStr">
+        <is>
+          <t>biały</t>
+        </is>
+      </c>
+      <c r="E10" s="7" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="n"/>
+      <c r="B11" s="7" t="n"/>
+      <c r="C11" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
         <is>
           <t>czarny</t>
         </is>
       </c>
-      <c r="E6" s="7" t="n"/>
-    </row>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
+      <c r="E11" s="7" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statyw metalowy</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E12" s="7" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="n"/>
+      <c r="B13" s="7" t="n"/>
+      <c r="C13" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E13" s="7" t="n"/>
+    </row>
     <row r="14"/>
     <row r="15"/>
     <row r="16"/>
@@ -544,12 +646,18 @@
     <row r="36"/>
     <row r="37"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade init method in order manager
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -407,7 +407,7 @@
     <row customHeight="1" ht="30" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>fimra01</t>
+          <t>sdasd</t>
         </is>
       </c>
     </row>
@@ -419,7 +419,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>22.4.2020</t>
+          <t>29.4.2020</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -429,7 +429,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>assdff123</t>
+          <t>ssaa22</t>
         </is>
       </c>
     </row>
@@ -441,7 +441,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>30.4.2020</t>
+          <t>29.4.2020</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -450,7 +450,7 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>123</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -487,10 +487,10 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
@@ -499,128 +499,14 @@
       </c>
       <c r="E5" s="7" t="n"/>
     </row>
-    <row r="6">
-      <c r="A6" s="7" t="n"/>
-      <c r="B6" s="7" t="n"/>
-      <c r="C6" s="6" t="n">
-        <v>32</v>
-      </c>
-      <c r="D6" s="5" t="inlineStr">
-        <is>
-          <t>czarny</t>
-        </is>
-      </c>
-      <c r="E6" s="7" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="n"/>
-      <c r="B7" s="7" t="n"/>
-      <c r="C7" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>bialy</t>
-        </is>
-      </c>
-      <c r="E7" s="7" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t>M3</t>
-        </is>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>styropian</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="n"/>
-      <c r="B9" s="7" t="n"/>
-      <c r="C9" s="6" t="n">
-        <v>32</v>
-      </c>
-      <c r="D9" s="5" t="inlineStr">
-        <is>
-          <t>czarny</t>
-        </is>
-      </c>
-      <c r="E9" s="7" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Statyw drewniany</t>
-        </is>
-      </c>
-      <c r="B10" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="C10" s="6" t="n">
-        <v>33</v>
-      </c>
-      <c r="D10" s="5" t="inlineStr">
-        <is>
-          <t>biały</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="7" t="n"/>
-      <c r="B11" s="7" t="n"/>
-      <c r="C11" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5" t="inlineStr">
-        <is>
-          <t>czarny</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Statyw metalowy</t>
-        </is>
-      </c>
-      <c r="B12" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="D12" s="5" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="E12" s="7" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="n"/>
-      <c r="B13" s="7" t="n"/>
-      <c r="C13" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
-      </c>
-      <c r="E13" s="7" t="n"/>
-    </row>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
     <row r="14"/>
     <row r="15"/>
     <row r="16"/>
@@ -646,18 +532,12 @@
     <row r="36"/>
     <row r="37"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B5"/>
+    <mergeCell ref="A5"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Name of PDFs changed
Now name of every PDF is connected with order date and company name
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -407,7 +407,7 @@
     <row customHeight="1" ht="30" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>sdasd</t>
+          <t>FIRMA2</t>
         </is>
       </c>
     </row>
@@ -419,7 +419,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>29.4.2020</t>
+          <t>13.5.2020</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -427,11 +427,7 @@
           <t xml:space="preserve">Nr faktury: </t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>ssaa22</t>
-        </is>
-      </c>
+      <c r="E2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -441,7 +437,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>29.4.2020</t>
+          <t>14.4.2020</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -450,7 +446,7 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0</v>
+        <v>2567</v>
       </c>
     </row>
     <row r="4">
@@ -483,32 +479,176 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
+          <t>D11</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>241</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>styropian</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="n"/>
+      <c r="B6" s="7" t="n"/>
+      <c r="C6" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>ecru</t>
+        </is>
+      </c>
+      <c r="E6" s="7" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="n"/>
+      <c r="B7" s="7" t="n"/>
+      <c r="C7" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>czerwony</t>
+        </is>
+      </c>
+      <c r="E7" s="7" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="n"/>
+      <c r="B8" s="7" t="n"/>
+      <c r="C8" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>czarny</t>
+        </is>
+      </c>
+      <c r="E8" s="7" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>73</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>styropian</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="n"/>
+      <c r="B10" s="7" t="n"/>
+      <c r="C10" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="D10" s="5" t="inlineStr">
+        <is>
+          <t>czarny</t>
+        </is>
+      </c>
+      <c r="E10" s="7" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
           <t>M1</t>
         </is>
       </c>
-      <c r="B5" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="B11" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
         <is>
           <t>styropian</t>
         </is>
       </c>
-      <c r="E5" s="7" t="n"/>
-    </row>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
+      <c r="E11" s="7" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statyw metalowy</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>110</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>Ślimak</t>
+        </is>
+      </c>
+      <c r="E12" s="7" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="n"/>
+      <c r="B13" s="7" t="n"/>
+      <c r="C13" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E13" s="7" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>Statyw drewniany</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="C14" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>biały</t>
+        </is>
+      </c>
+      <c r="E14" s="7" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="n"/>
+      <c r="B15" s="7" t="n"/>
+      <c r="C15" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D15" s="5" t="inlineStr">
+        <is>
+          <t>naturalny</t>
+        </is>
+      </c>
+      <c r="E15" s="7" t="n"/>
+    </row>
     <row r="16"/>
     <row r="17"/>
     <row r="18"/>
@@ -532,12 +672,20 @@
     <row r="36"/>
     <row r="37"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="13">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5"/>
-    <mergeCell ref="A5"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B11"/>
+    <mergeCell ref="A11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Sort PDF in main folder
- create in main folder, subfolders which gather all year orders. Inside every year folder there are folders with orders from each month
</commit_message>
<xml_diff>
--- a/tkinter_test.xlsx
+++ b/tkinter_test.xlsx
@@ -407,7 +407,7 @@
     <row customHeight="1" ht="30" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>FIRMA2</t>
+          <t>firma54</t>
         </is>
       </c>
     </row>
@@ -419,7 +419,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>13.5.2020</t>
+          <t>19.3.2020</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -427,7 +427,11 @@
           <t xml:space="preserve">Nr faktury: </t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr"/>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>ec22/2020</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -437,7 +441,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>14.4.2020</t>
+          <t>1.1.1</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -446,7 +450,7 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>2567</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -479,11 +483,11 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>D11</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>241</v>
+        <v>78</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>12</v>
@@ -499,11 +503,11 @@
       <c r="A6" s="7" t="n"/>
       <c r="B6" s="7" t="n"/>
       <c r="C6" s="6" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
-          <t>ecru</t>
+          <t>czarny</t>
         </is>
       </c>
       <c r="E6" s="7" t="n"/>
@@ -512,24 +516,30 @@
       <c r="A7" s="7" t="n"/>
       <c r="B7" s="7" t="n"/>
       <c r="C7" s="6" t="n">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>czerwony</t>
+          <t>bialy</t>
         </is>
       </c>
       <c r="E7" s="7" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="n"/>
-      <c r="B8" s="7" t="n"/>
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>Statyw metalowy</t>
+        </is>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>33</v>
+      </c>
       <c r="C8" s="6" t="n">
-        <v>150</v>
+        <v>33</v>
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>czarny</t>
+          <t>90</t>
         </is>
       </c>
       <c r="E8" s="7" t="n"/>
@@ -537,18 +547,18 @@
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>Akcesoria</t>
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
-          <t>styropian</t>
+          <t>trzpień</t>
         </is>
       </c>
       <c r="E9" s="7" t="n"/>
@@ -557,11 +567,11 @@
       <c r="A10" s="7" t="n"/>
       <c r="B10" s="7" t="n"/>
       <c r="C10" s="6" t="n">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D10" s="5" t="inlineStr">
         <is>
-          <t>czarny</t>
+          <t>trzpień</t>
         </is>
       </c>
       <c r="E10" s="7" t="n"/>
@@ -569,86 +579,38 @@
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>M1</t>
+          <t>Statyw drewniany</t>
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>50</v>
+        <v>567</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="D11" s="5" t="inlineStr">
         <is>
-          <t>styropian</t>
+          <t>biały</t>
         </is>
       </c>
       <c r="E11" s="7" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Statyw metalowy</t>
-        </is>
-      </c>
-      <c r="B12" s="5" t="n">
-        <v>110</v>
-      </c>
+      <c r="A12" s="7" t="n"/>
+      <c r="B12" s="7" t="n"/>
       <c r="C12" s="6" t="n">
-        <v>60</v>
+        <v>555</v>
       </c>
       <c r="D12" s="5" t="inlineStr">
         <is>
-          <t>Ślimak</t>
+          <t>czarny</t>
         </is>
       </c>
       <c r="E12" s="7" t="n"/>
     </row>
-    <row r="13">
-      <c r="A13" s="7" t="n"/>
-      <c r="B13" s="7" t="n"/>
-      <c r="C13" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="D13" s="5" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
-      </c>
-      <c r="E13" s="7" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>Statyw drewniany</t>
-        </is>
-      </c>
-      <c r="B14" s="5" t="n">
-        <v>70</v>
-      </c>
-      <c r="C14" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="D14" s="5" t="inlineStr">
-        <is>
-          <t>biały</t>
-        </is>
-      </c>
-      <c r="E14" s="7" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="7" t="n"/>
-      <c r="B15" s="7" t="n"/>
-      <c r="C15" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="D15" s="5" t="inlineStr">
-        <is>
-          <t>naturalny</t>
-        </is>
-      </c>
-      <c r="E15" s="7" t="n"/>
-    </row>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
     <row r="16"/>
     <row r="17"/>
     <row r="18"/>
@@ -672,20 +634,18 @@
     <row r="36"/>
     <row r="37"/>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="11">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B8"/>
+    <mergeCell ref="A8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B11"/>
-    <mergeCell ref="A11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>